<commit_message>
update auto put student into class
update auto put student into class
</commit_message>
<xml_diff>
--- a/Database/Data_20150722/Class2.xlsx
+++ b/Database/Data_20150722/Class2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="42">
   <si>
     <t>Class</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>IA</t>
-  </si>
-  <si>
-    <t>IA1</t>
   </si>
 </sst>
 </file>
@@ -567,7 +564,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1290,7 @@
         <v>29</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F28">
         <v>9</v>

</xml_diff>